<commit_message>
Added DCF for NVDA - Need to add Street Predictions for Rev, Etc
</commit_message>
<xml_diff>
--- a/NVDA DCF.xlsx
+++ b/NVDA DCF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gus-c\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB830A0-8E3A-4A60-9E5D-A523FE49137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD213E0B-7BB4-4F61-B1FF-3CF177369306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{7C0A4711-C170-4708-A88B-4ECCC81C6516}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C0A4711-C170-4708-A88B-4ECCC81C6516}"/>
   </bookViews>
   <sheets>
     <sheet name="DCF" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="217">
   <si>
     <t>NVIDIA Corporation (NVDA)</t>
   </si>
@@ -682,6 +682,12 @@
   </si>
   <si>
     <t>NVDA 67066 2379504 NASDAQ Common stock (FactSet Dataset)</t>
+  </si>
+  <si>
+    <t>Future Years Lacking Street Predictions from Brokers</t>
+  </si>
+  <si>
+    <t>del</t>
   </si>
 </sst>
 </file>
@@ -1434,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C967E1C5-2521-4EC3-8FBA-A340B4830478}">
   <dimension ref="B2:AG75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1468,6 +1474,9 @@
       <c r="K2" s="7" t="s">
         <v>204</v>
       </c>
+      <c r="O2" s="7" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
@@ -1931,6 +1940,9 @@
       <c r="N20" s="35">
         <f>Financials!Y18</f>
         <v>10041000000</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.2">
@@ -11172,7 +11184,7 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="11" ySplit="8" topLeftCell="L9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>

</xml_diff>